<commit_message>
Check in auto and fix to the user controls
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19740" windowHeight="5910" xr2:uid="{84364B8A-653F-400C-BF42-269DA731DB7B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19740" windowHeight="5910" activeTab="1" xr2:uid="{84364B8A-653F-400C-BF42-269DA731DB7B}"/>
   </bookViews>
   <sheets>
     <sheet name="RawPoints" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="117">
   <si>
     <t>FieldXRedWall</t>
   </si>
@@ -370,6 +370,12 @@
   </si>
   <si>
     <t>Bad</t>
+  </si>
+  <si>
+    <t>Move8</t>
+  </si>
+  <si>
+    <t>Move eight feet</t>
   </si>
 </sst>
 </file>
@@ -385,12 +391,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -405,9 +417,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -726,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDDAE613-BBFC-4F5C-AD8E-7A070BBCC1B5}">
   <dimension ref="B1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection sqref="A1:H35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +787,7 @@
       </c>
       <c r="H3">
         <f>C10+C4</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -791,7 +807,7 @@
       </c>
       <c r="H4">
         <f>C18-C4</f>
-        <v>88.25</v>
+        <v>208.25</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -811,7 +827,7 @@
       </c>
       <c r="H5">
         <f>C19-C4</f>
-        <v>136.25</v>
+        <v>160.25</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -850,7 +866,7 @@
       </c>
       <c r="H7">
         <f>C11-C4</f>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -858,7 +874,7 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>324</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -866,8 +882,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <f>24*12</f>
-        <v>288</v>
+        <v>0</v>
       </c>
       <c r="F9" t="s">
         <v>35</v>
@@ -878,7 +893,7 @@
       </c>
       <c r="H9">
         <f>H3</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -886,8 +901,8 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <f>C8+30</f>
-        <v>30</v>
+        <f>C8-30</f>
+        <v>294</v>
       </c>
       <c r="F10" t="s">
         <v>39</v>
@@ -898,7 +913,7 @@
       </c>
       <c r="H10">
         <f t="shared" ref="H10:H13" si="0">H4</f>
-        <v>88.25</v>
+        <v>208.25</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -906,8 +921,8 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <f>C9-30</f>
-        <v>258</v>
+        <f>C9+30</f>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
         <v>36</v>
@@ -918,7 +933,7 @@
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>136.25</v>
+        <v>160.25</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -958,7 +973,7 @@
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -987,7 +1002,7 @@
       </c>
       <c r="H15">
         <f>C21-C5</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -1007,7 +1022,7 @@
       </c>
       <c r="H16">
         <f>H15</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -1027,7 +1042,7 @@
       </c>
       <c r="H17">
         <f>C22-C4</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -1035,6 +1050,10 @@
         <v>19</v>
       </c>
       <c r="C18">
+        <v>222</v>
+      </c>
+      <c r="D18">
+        <f>324-C18</f>
         <v>102</v>
       </c>
       <c r="F18" t="s">
@@ -1046,7 +1065,7 @@
       </c>
       <c r="H18">
         <f>H17</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1054,6 +1073,10 @@
         <v>20</v>
       </c>
       <c r="C19">
+        <v>174</v>
+      </c>
+      <c r="D19">
+        <f>324-C19</f>
         <v>150</v>
       </c>
       <c r="F19" t="s">
@@ -1065,7 +1088,7 @@
       </c>
       <c r="H19">
         <f>H20-C20</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1084,7 +1107,7 @@
       </c>
       <c r="H20">
         <f>C21-C5</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1092,6 +1115,10 @@
         <v>22</v>
       </c>
       <c r="C21">
+        <v>238.75</v>
+      </c>
+      <c r="D21">
+        <f>324-C21</f>
         <v>85.25</v>
       </c>
       <c r="F21" t="s">
@@ -1103,7 +1130,7 @@
       </c>
       <c r="H21">
         <f>H22+C20</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -1111,8 +1138,8 @@
         <v>23</v>
       </c>
       <c r="C22">
-        <f>C9-C21</f>
-        <v>202.75</v>
+        <f>C8-C21</f>
+        <v>85.25</v>
       </c>
       <c r="F22" t="s">
         <v>34</v>
@@ -1123,7 +1150,7 @@
       </c>
       <c r="H22">
         <f>C22+C5</f>
-        <v>218.75</v>
+        <v>101.25</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -1142,7 +1169,7 @@
       </c>
       <c r="H23">
         <f>H15</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1161,7 +1188,7 @@
       </c>
       <c r="H24">
         <f>H16</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1169,6 +1196,10 @@
         <v>90</v>
       </c>
       <c r="C25">
+        <v>252.43</v>
+      </c>
+      <c r="D25">
+        <f>324-C25</f>
         <v>71.569999999999993</v>
       </c>
       <c r="F25" t="s">
@@ -1180,7 +1211,7 @@
       </c>
       <c r="H25">
         <f>H17</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -1188,6 +1219,10 @@
         <v>91</v>
       </c>
       <c r="C26">
+        <v>217.75</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ref="D26:D28" si="1">324-C26</f>
         <v>106.25</v>
       </c>
       <c r="F26" t="s">
@@ -1199,7 +1234,7 @@
       </c>
       <c r="H26">
         <f>H18</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -1207,6 +1242,10 @@
         <v>92</v>
       </c>
       <c r="C27">
+        <v>71.569999999999993</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
         <v>252.43</v>
       </c>
       <c r="F27" t="s">
@@ -1218,7 +1257,7 @@
       </c>
       <c r="H27">
         <f>H28-C20</f>
-        <v>59.569999999999993</v>
+        <v>240.43</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -1226,6 +1265,10 @@
         <v>93</v>
       </c>
       <c r="C28">
+        <v>107.57</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
         <v>216.43</v>
       </c>
       <c r="F28" t="s">
@@ -1237,7 +1280,7 @@
       </c>
       <c r="H28">
         <f>C25</f>
-        <v>71.569999999999993</v>
+        <v>252.43</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -1250,7 +1293,7 @@
       </c>
       <c r="H29">
         <f>H30+C20</f>
-        <v>264.43</v>
+        <v>83.57</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -1263,7 +1306,7 @@
       </c>
       <c r="H30">
         <f>C27</f>
-        <v>252.43</v>
+        <v>71.569999999999993</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -1276,7 +1319,7 @@
       </c>
       <c r="H31">
         <f>C26-C4</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -1289,7 +1332,7 @@
       </c>
       <c r="H32">
         <f>H31</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.25">
@@ -1302,7 +1345,7 @@
       </c>
       <c r="H33">
         <f>C28+C4</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.25">
@@ -1315,7 +1358,7 @@
       </c>
       <c r="H34">
         <f>H33</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.25">
@@ -1336,10 +1379,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B2C6CC-E6B0-438C-8DA4-A8209BB034F1}">
-  <dimension ref="A1:R31"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,7 +1464,7 @@
       </c>
       <c r="E2" s="1">
         <f>RawPoints!H4</f>
-        <v>88.25</v>
+        <v>208.25</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -1432,7 +1475,7 @@
       </c>
       <c r="H2" s="1">
         <f>RawPoints!H15</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
       <c r="I2" s="1">
         <v>0</v>
@@ -1443,7 +1486,7 @@
       </c>
       <c r="K2" s="1">
         <f>RawPoints!H16</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
       <c r="L2" s="1">
         <v>0</v>
@@ -1465,7 +1508,7 @@
       </c>
       <c r="E3" s="1">
         <f>E2</f>
-        <v>88.25</v>
+        <v>208.25</v>
       </c>
       <c r="F3" s="1">
         <f>F2</f>
@@ -1477,7 +1520,7 @@
       </c>
       <c r="H3" s="1">
         <f>RawPoints!H17</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -1488,57 +1531,63 @@
       </c>
       <c r="K3" s="1">
         <f>H3</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="L3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
         <f>D2</f>
         <v>16</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
         <f>RawPoints!H5</f>
-        <v>136.25</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <f>G2</f>
+        <v>160.25</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" ref="G4:L4" si="0">G2</f>
         <v>112</v>
       </c>
-      <c r="H4" s="1">
-        <f>H2</f>
-        <v>69.25</v>
-      </c>
-      <c r="I4" s="1">
-        <f>I2</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <f>J2</f>
+      <c r="H4" s="3">
+        <f t="shared" si="0"/>
+        <v>222.75</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="0"/>
         <v>124</v>
       </c>
-      <c r="K4" s="1">
-        <f>K2</f>
-        <v>69.25</v>
-      </c>
-      <c r="L4" s="1">
-        <f>L2</f>
-        <v>0</v>
-      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="0"/>
+        <v>222.75</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1556,7 +1605,7 @@
       </c>
       <c r="E5" s="1">
         <f>E4</f>
-        <v>136.25</v>
+        <v>160.25</v>
       </c>
       <c r="F5" s="1">
         <f>F4</f>
@@ -1568,7 +1617,7 @@
       </c>
       <c r="H5" s="1">
         <f>H3</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="I5" s="1">
         <f>I4</f>
@@ -1580,7 +1629,7 @@
       </c>
       <c r="K5" s="1">
         <f>K3</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="L5" s="1">
         <f>L4</f>
@@ -1614,23 +1663,23 @@
         <v>112</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" ref="H6:L8" si="0">H4</f>
-        <v>69.25</v>
+        <f t="shared" ref="H6:L8" si="1">H4</f>
+        <v>222.75</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>124</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="0"/>
-        <v>69.25</v>
+        <f t="shared" si="1"/>
+        <v>222.75</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1657,27 +1706,27 @@
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" ref="G7:L7" si="1">G5</f>
+        <f t="shared" ref="G7:L7" si="2">G5</f>
         <v>112</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="1"/>
-        <v>189</v>
+        <f t="shared" si="2"/>
+        <v>71.5</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>124</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="1"/>
-        <v>189</v>
+        <f t="shared" si="2"/>
+        <v>71.5</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1697,7 +1746,7 @@
       </c>
       <c r="E8" s="1">
         <f>RawPoints!H3</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
       <c r="F8" s="1">
         <f>F7</f>
@@ -1708,23 +1757,23 @@
         <v>112</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="0"/>
-        <v>69.25</v>
+        <f t="shared" si="1"/>
+        <v>222.75</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>124</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="0"/>
-        <v>69.25</v>
+        <f t="shared" si="1"/>
+        <v>222.75</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1744,7 +1793,7 @@
       </c>
       <c r="E9" s="1">
         <f>E8</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
       <c r="F9" s="1">
         <f>F8</f>
@@ -1756,7 +1805,7 @@
       </c>
       <c r="H9" s="1">
         <f>RawPoints!H19</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I9" s="1">
         <v>75</v>
@@ -1767,7 +1816,7 @@
       </c>
       <c r="K9" s="1">
         <f>RawPoints!H20</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
       <c r="L9" s="1">
         <v>90</v>
@@ -1789,7 +1838,7 @@
       </c>
       <c r="E10" s="1">
         <f>RawPoints!H7</f>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -1800,7 +1849,7 @@
       </c>
       <c r="H10" s="1">
         <f>RawPoints!H21</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I10" s="1">
         <v>-75</v>
@@ -1811,7 +1860,7 @@
       </c>
       <c r="K10" s="1">
         <f>RawPoints!H22</f>
-        <v>218.75</v>
+        <v>101.25</v>
       </c>
       <c r="L10" s="1">
         <v>-90</v>
@@ -1833,7 +1882,7 @@
       </c>
       <c r="E11" s="1">
         <f>E2</f>
-        <v>88.25</v>
+        <v>208.25</v>
       </c>
       <c r="F11" s="1">
         <f>F10</f>
@@ -1844,7 +1893,7 @@
       </c>
       <c r="H11" s="1">
         <f>K11</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I11" s="1">
         <v>-25</v>
@@ -1855,7 +1904,7 @@
       </c>
       <c r="K11" s="1">
         <f>H9</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="L11" s="1">
         <v>25</v>
@@ -1866,7 +1915,7 @@
       </c>
       <c r="N11" s="1">
         <f>K9</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
       <c r="O11" s="1">
         <v>90</v>
@@ -1898,7 +1947,7 @@
       </c>
       <c r="H12" s="1">
         <f>H10</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I12" s="1">
         <v>25</v>
@@ -1909,7 +1958,7 @@
       </c>
       <c r="K12" s="1">
         <f>H10</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="L12" s="1">
         <v>-25</v>
@@ -1920,7 +1969,7 @@
       </c>
       <c r="N12" s="1">
         <f>K10</f>
-        <v>218.75</v>
+        <v>101.25</v>
       </c>
       <c r="O12" s="1">
         <v>-90</v>
@@ -1942,7 +1991,7 @@
       </c>
       <c r="E13" s="1">
         <f>E8</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -1953,7 +2002,7 @@
       </c>
       <c r="H13" s="1">
         <f>H11</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I13" s="1">
         <v>-25</v>
@@ -1964,7 +2013,7 @@
       </c>
       <c r="K13" s="1">
         <f>H13</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="L13" s="1">
         <v>25</v>
@@ -1975,7 +2024,7 @@
       </c>
       <c r="N13" s="1">
         <f>RawPoints!H23</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
       <c r="O13" s="1">
         <v>125</v>
@@ -1986,7 +2035,7 @@
       </c>
       <c r="Q13" s="1">
         <f>RawPoints!H24</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
       <c r="R13" s="1">
         <v>180</v>
@@ -2008,7 +2057,7 @@
       </c>
       <c r="E14" s="1">
         <f>E2</f>
-        <v>88.25</v>
+        <v>208.25</v>
       </c>
       <c r="F14" s="1">
         <f>F13</f>
@@ -2020,18 +2069,18 @@
       </c>
       <c r="H14" s="1">
         <f>H13</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I14" s="1">
         <v>-25</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" ref="J14:J16" si="2">M14</f>
+        <f t="shared" ref="J14:J16" si="3">M14</f>
         <v>208</v>
       </c>
       <c r="K14" s="1">
         <f>H14</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="L14" s="1">
         <v>25</v>
@@ -2041,20 +2090,20 @@
         <v>208</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" ref="N14:R14" si="3">N13</f>
-        <v>69.25</v>
+        <f t="shared" ref="N14:Q14" si="4">N13</f>
+        <v>222.75</v>
       </c>
       <c r="O14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>125</v>
       </c>
       <c r="P14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>196</v>
       </c>
       <c r="Q14" s="1">
-        <f t="shared" si="3"/>
-        <v>69.25</v>
+        <f t="shared" si="4"/>
+        <v>222.75</v>
       </c>
       <c r="R14" s="1">
         <v>180</v>
@@ -2086,18 +2135,18 @@
       </c>
       <c r="H15" s="1">
         <f>H12</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I15" s="1">
         <v>25</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>208</v>
       </c>
       <c r="K15" s="1">
         <f>H15</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="L15" s="1">
         <v>-25</v>
@@ -2108,7 +2157,7 @@
       </c>
       <c r="N15" s="1">
         <f>RawPoints!H25</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="O15" s="1">
         <v>-125</v>
@@ -2119,7 +2168,7 @@
       </c>
       <c r="Q15" s="1">
         <f>N15</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="R15" s="1">
         <v>180</v>
@@ -2141,7 +2190,7 @@
       </c>
       <c r="E16" s="1">
         <f>E10</f>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -2151,18 +2200,18 @@
       </c>
       <c r="H16" s="1">
         <f>H12</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I16" s="1">
         <v>25</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>208</v>
       </c>
       <c r="K16" s="1">
         <f>H16</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="L16" s="1">
         <v>-25</v>
@@ -2173,7 +2222,7 @@
       </c>
       <c r="N16" s="1">
         <f>N15</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="O16" s="1">
         <v>-125</v>
@@ -2184,7 +2233,7 @@
       </c>
       <c r="Q16" s="1">
         <f>Q15</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="R16" s="1">
         <v>180</v>
@@ -2206,7 +2255,7 @@
       </c>
       <c r="E17" s="1">
         <f>E16</f>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -2217,7 +2266,7 @@
       </c>
       <c r="H17" s="1">
         <f>H7</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="I17" s="1">
         <f>I8</f>
@@ -2229,7 +2278,7 @@
       </c>
       <c r="K17" s="1">
         <f>K7</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="L17" s="1">
         <f>L8</f>
@@ -2252,7 +2301,7 @@
       </c>
       <c r="E18" s="1">
         <f>E8</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
       <c r="F18" s="1">
         <f>F17</f>
@@ -2264,7 +2313,7 @@
       </c>
       <c r="H18" s="1">
         <f>H14</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I18" s="1">
         <v>-25</v>
@@ -2275,7 +2324,7 @@
       </c>
       <c r="K18" s="1">
         <f>RawPoints!H27</f>
-        <v>59.569999999999993</v>
+        <v>240.43</v>
       </c>
       <c r="L18" s="1">
         <v>25</v>
@@ -2286,7 +2335,7 @@
       </c>
       <c r="N18" s="1">
         <f>RawPoints!H28</f>
-        <v>71.569999999999993</v>
+        <v>252.43</v>
       </c>
       <c r="O18" s="1">
         <v>90</v>
@@ -2303,24 +2352,24 @@
         <v>5</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" ref="D19:D29" si="4">D18</f>
+        <f t="shared" ref="D19:D29" si="5">D18</f>
         <v>16</v>
       </c>
       <c r="E19" s="1">
         <f>E18</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" ref="F19:F25" si="5">F18</f>
+        <f t="shared" ref="F19:F25" si="6">F18</f>
         <v>0</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" ref="G19:G25" si="6">G16</f>
+        <f t="shared" ref="G19:G25" si="7">G16</f>
         <v>140</v>
       </c>
       <c r="H19" s="1">
         <f>H18</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I19" s="1">
         <f>I18</f>
@@ -2332,7 +2381,7 @@
       </c>
       <c r="K19" s="1">
         <f>H19</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="L19" s="1">
         <v>25</v>
@@ -2343,7 +2392,7 @@
       </c>
       <c r="N19" s="1">
         <f>RawPoints!H31</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
       <c r="O19" s="1">
         <v>45</v>
@@ -2354,7 +2403,7 @@
       </c>
       <c r="Q19" s="1">
         <f>N19</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
       <c r="R19" s="1">
         <v>0</v>
@@ -2371,15 +2420,15 @@
         <v>4</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E20" s="1">
         <f>E2</f>
-        <v>88.25</v>
+        <v>208.25</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G20" s="1">
@@ -2388,7 +2437,7 @@
       </c>
       <c r="H20" s="1">
         <f>H19</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I20" s="1">
         <v>25</v>
@@ -2399,21 +2448,21 @@
       </c>
       <c r="K20" s="1">
         <f>K18</f>
-        <v>59.569999999999993</v>
+        <v>240.43</v>
       </c>
       <c r="L20" s="1">
         <v>-25</v>
       </c>
       <c r="M20" s="1">
-        <f>M18</f>
+        <f t="shared" ref="M20:O21" si="8">M18</f>
         <v>324</v>
       </c>
       <c r="N20" s="1">
-        <f>N18</f>
-        <v>71.569999999999993</v>
+        <f t="shared" si="8"/>
+        <v>252.43</v>
       </c>
       <c r="O20" s="1">
-        <f>O18</f>
+        <f t="shared" si="8"/>
         <v>90</v>
       </c>
     </row>
@@ -2428,24 +2477,24 @@
         <v>5</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E21" s="1">
         <f>E20</f>
-        <v>88.25</v>
+        <v>208.25</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>140</v>
       </c>
       <c r="H21" s="1">
         <f>H20</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I21" s="1">
         <f>I20</f>
@@ -2457,21 +2506,21 @@
       </c>
       <c r="K21" s="1">
         <f>H21</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="L21" s="1">
         <v>-25</v>
       </c>
       <c r="M21" s="1">
-        <f>M19</f>
+        <f t="shared" si="8"/>
         <v>288</v>
       </c>
       <c r="N21" s="1">
-        <f>N19</f>
-        <v>92.5</v>
+        <f t="shared" si="8"/>
+        <v>204</v>
       </c>
       <c r="O21" s="1">
-        <f>O19</f>
+        <f t="shared" si="8"/>
         <v>45</v>
       </c>
       <c r="P21" s="1">
@@ -2480,7 +2529,7 @@
       </c>
       <c r="Q21" s="1">
         <f>Q19</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
       <c r="R21" s="1">
         <f>R19</f>
@@ -2498,7 +2547,7 @@
         <v>4</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E22" s="1">
@@ -2506,16 +2555,16 @@
         <v>182.25</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>140</v>
       </c>
       <c r="H22" s="1">
         <f>H15</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I22" s="1">
         <v>25</v>
@@ -2526,7 +2575,7 @@
       </c>
       <c r="K22" s="1">
         <f>RawPoints!H29</f>
-        <v>264.43</v>
+        <v>83.57</v>
       </c>
       <c r="L22" s="1">
         <v>-25</v>
@@ -2537,7 +2586,7 @@
       </c>
       <c r="N22" s="1">
         <f>RawPoints!H30</f>
-        <v>252.43</v>
+        <v>71.569999999999993</v>
       </c>
       <c r="O22" s="1">
         <v>-90</v>
@@ -2554,7 +2603,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E23" s="1">
@@ -2562,7 +2611,7 @@
         <v>182.25</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G23" s="1">
@@ -2571,7 +2620,7 @@
       </c>
       <c r="H23" s="1">
         <f>H22</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I23" s="1">
         <f>I22</f>
@@ -2583,7 +2632,7 @@
       </c>
       <c r="K23" s="1">
         <f>H23</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="L23" s="1">
         <v>-25</v>
@@ -2594,7 +2643,7 @@
       </c>
       <c r="N23" s="1">
         <f>RawPoints!H33</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
       <c r="O23" s="1">
         <v>-90</v>
@@ -2605,7 +2654,7 @@
       </c>
       <c r="Q23" s="1">
         <f>N23</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
       <c r="R23" s="1">
         <v>0</v>
@@ -2622,24 +2671,24 @@
         <v>4</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E24" s="1">
         <f>E16</f>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>140</v>
       </c>
       <c r="H24" s="1">
         <f>H23</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I24" s="1">
         <f>I23</f>
@@ -2651,7 +2700,7 @@
       </c>
       <c r="K24" s="1">
         <f>K22</f>
-        <v>264.43</v>
+        <v>83.57</v>
       </c>
       <c r="L24" s="1">
         <v>-75</v>
@@ -2662,7 +2711,7 @@
       </c>
       <c r="N24" s="1">
         <f>N22</f>
-        <v>252.43</v>
+        <v>71.569999999999993</v>
       </c>
       <c r="O24" s="1">
         <v>-90</v>
@@ -2679,24 +2728,24 @@
         <v>5</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E25" s="1">
         <f>E24</f>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>140</v>
       </c>
       <c r="H25" s="1">
         <f>H24</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I25" s="1">
         <f>I24</f>
@@ -2708,7 +2757,7 @@
       </c>
       <c r="K25" s="1">
         <f>H25</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="L25" s="1">
         <v>-75</v>
@@ -2719,7 +2768,7 @@
       </c>
       <c r="N25" s="1">
         <f>N23</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
       <c r="O25" s="1">
         <f>O23</f>
@@ -2731,7 +2780,7 @@
       </c>
       <c r="Q25" s="1">
         <f>Q23</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
       <c r="R25" s="1">
         <f>R23</f>
@@ -2749,12 +2798,12 @@
         <v>5</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E26" s="1">
         <f>E18</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -2765,7 +2814,7 @@
       </c>
       <c r="H26" s="1">
         <f>H20</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I26" s="1">
         <v>-25</v>
@@ -2776,7 +2825,7 @@
       </c>
       <c r="K26" s="1">
         <f>H26</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="L26" s="1">
         <v>25</v>
@@ -2787,7 +2836,7 @@
       </c>
       <c r="N26" s="1">
         <f>N23</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
       <c r="O26" s="1">
         <v>-25</v>
@@ -2798,7 +2847,7 @@
       </c>
       <c r="Q26" s="1">
         <f>Q25</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
       <c r="R26" s="1">
         <f>R25</f>
@@ -2816,23 +2865,23 @@
         <v>5</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E27" s="1">
         <f>E26</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" ref="G27:G29" si="7">G26</f>
+        <f t="shared" ref="G27:G29" si="9">G26</f>
         <v>140</v>
       </c>
       <c r="H27" s="1">
         <f>H26</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I27" s="1">
         <v>-25</v>
@@ -2843,7 +2892,7 @@
       </c>
       <c r="K27" s="1">
         <f>H27</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="L27" s="1">
         <v>25</v>
@@ -2854,7 +2903,7 @@
       </c>
       <c r="N27" s="1">
         <f>N26</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
       <c r="O27" s="1">
         <v>-25</v>
@@ -2865,7 +2914,7 @@
       </c>
       <c r="Q27" s="1">
         <f>Q26</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
       <c r="R27" s="1">
         <f>R26</f>
@@ -2883,34 +2932,34 @@
         <v>5</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E28" s="1">
         <f>E24</f>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
       </c>
       <c r="G28" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>140</v>
       </c>
       <c r="H28" s="1">
         <f>H25</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I28" s="1">
         <v>25</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" ref="J28:J29" si="8">J27</f>
+        <f t="shared" ref="J28:J29" si="10">J27</f>
         <v>228.75</v>
       </c>
       <c r="K28" s="1">
         <f>K23</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="L28" s="1">
         <v>-25</v>
@@ -2921,7 +2970,7 @@
       </c>
       <c r="N28" s="1">
         <f>N21</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
       <c r="O28" s="1">
         <v>25</v>
@@ -2932,7 +2981,7 @@
       </c>
       <c r="Q28" s="1">
         <f>Q21</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
       <c r="R28" s="1">
         <v>0</v>
@@ -2949,35 +2998,35 @@
         <v>5</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E29" s="1">
         <f>E25</f>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
       </c>
       <c r="G29" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>140</v>
       </c>
       <c r="H29" s="1">
         <f>H28</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I29" s="1">
         <f>I25</f>
         <v>25</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>228.75</v>
       </c>
       <c r="K29" s="1">
         <f>H29</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="L29" s="1">
         <f>L28</f>
@@ -2989,7 +3038,7 @@
       </c>
       <c r="N29" s="1">
         <f>N28</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
       <c r="O29" s="1">
         <v>25</v>
@@ -3000,7 +3049,7 @@
       </c>
       <c r="Q29" s="1">
         <f>N29</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
       <c r="R29" s="1">
         <v>0</v>
@@ -3037,10 +3086,10 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B31" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -3055,12 +3104,41 @@
         <v>0</v>
       </c>
       <c r="G31" s="1">
+        <v>96</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
         <v>120</v>
       </c>
-      <c r="H31" s="1">
-        <v>0</v>
-      </c>
-      <c r="I31" s="1">
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Check in auto and fix to the user controls"
This reverts commit cb8ffb34a8ffdace0f2aa01dbedc604de2d85f60.
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19740" windowHeight="5910" activeTab="1" xr2:uid="{84364B8A-653F-400C-BF42-269DA731DB7B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19740" windowHeight="5910" xr2:uid="{84364B8A-653F-400C-BF42-269DA731DB7B}"/>
   </bookViews>
   <sheets>
     <sheet name="RawPoints" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="115">
   <si>
     <t>FieldXRedWall</t>
   </si>
@@ -370,12 +370,6 @@
   </si>
   <si>
     <t>Bad</t>
-  </si>
-  <si>
-    <t>Move8</t>
-  </si>
-  <si>
-    <t>Move eight feet</t>
   </si>
 </sst>
 </file>
@@ -391,18 +385,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -417,13 +405,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -742,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDDAE613-BBFC-4F5C-AD8E-7A070BBCC1B5}">
   <dimension ref="B1:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection sqref="A1:H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,7 +771,7 @@
       </c>
       <c r="H3">
         <f>C10+C4</f>
-        <v>307.75</v>
+        <v>43.75</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -807,7 +791,7 @@
       </c>
       <c r="H4">
         <f>C18-C4</f>
-        <v>208.25</v>
+        <v>88.25</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -827,7 +811,7 @@
       </c>
       <c r="H5">
         <f>C19-C4</f>
-        <v>160.25</v>
+        <v>136.25</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -866,7 +850,7 @@
       </c>
       <c r="H7">
         <f>C11-C4</f>
-        <v>16.25</v>
+        <v>244.25</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -874,7 +858,7 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>324</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -882,7 +866,8 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <f>24*12</f>
+        <v>288</v>
       </c>
       <c r="F9" t="s">
         <v>35</v>
@@ -893,7 +878,7 @@
       </c>
       <c r="H9">
         <f>H3</f>
-        <v>307.75</v>
+        <v>43.75</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -901,8 +886,8 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <f>C8-30</f>
-        <v>294</v>
+        <f>C8+30</f>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
         <v>39</v>
@@ -913,7 +898,7 @@
       </c>
       <c r="H10">
         <f t="shared" ref="H10:H13" si="0">H4</f>
-        <v>208.25</v>
+        <v>88.25</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -921,8 +906,8 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <f>C9+30</f>
-        <v>30</v>
+        <f>C9-30</f>
+        <v>258</v>
       </c>
       <c r="F11" t="s">
         <v>36</v>
@@ -933,7 +918,7 @@
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>160.25</v>
+        <v>136.25</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -973,7 +958,7 @@
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>16.25</v>
+        <v>244.25</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -1002,7 +987,7 @@
       </c>
       <c r="H15">
         <f>C21-C5</f>
-        <v>222.75</v>
+        <v>69.25</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -1022,7 +1007,7 @@
       </c>
       <c r="H16">
         <f>H15</f>
-        <v>222.75</v>
+        <v>69.25</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -1042,7 +1027,7 @@
       </c>
       <c r="H17">
         <f>C22-C4</f>
-        <v>71.5</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -1050,10 +1035,6 @@
         <v>19</v>
       </c>
       <c r="C18">
-        <v>222</v>
-      </c>
-      <c r="D18">
-        <f>324-C18</f>
         <v>102</v>
       </c>
       <c r="F18" t="s">
@@ -1065,7 +1046,7 @@
       </c>
       <c r="H18">
         <f>H17</f>
-        <v>71.5</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1073,10 +1054,6 @@
         <v>20</v>
       </c>
       <c r="C19">
-        <v>174</v>
-      </c>
-      <c r="D19">
-        <f>324-C19</f>
         <v>150</v>
       </c>
       <c r="F19" t="s">
@@ -1088,7 +1065,7 @@
       </c>
       <c r="H19">
         <f>H20-C20</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1107,7 +1084,7 @@
       </c>
       <c r="H20">
         <f>C21-C5</f>
-        <v>222.75</v>
+        <v>69.25</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1115,10 +1092,6 @@
         <v>22</v>
       </c>
       <c r="C21">
-        <v>238.75</v>
-      </c>
-      <c r="D21">
-        <f>324-C21</f>
         <v>85.25</v>
       </c>
       <c r="F21" t="s">
@@ -1130,7 +1103,7 @@
       </c>
       <c r="H21">
         <f>H22+C20</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -1138,8 +1111,8 @@
         <v>23</v>
       </c>
       <c r="C22">
-        <f>C8-C21</f>
-        <v>85.25</v>
+        <f>C9-C21</f>
+        <v>202.75</v>
       </c>
       <c r="F22" t="s">
         <v>34</v>
@@ -1150,7 +1123,7 @@
       </c>
       <c r="H22">
         <f>C22+C5</f>
-        <v>101.25</v>
+        <v>218.75</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -1169,7 +1142,7 @@
       </c>
       <c r="H23">
         <f>H15</f>
-        <v>222.75</v>
+        <v>69.25</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1188,7 +1161,7 @@
       </c>
       <c r="H24">
         <f>H16</f>
-        <v>222.75</v>
+        <v>69.25</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1196,10 +1169,6 @@
         <v>90</v>
       </c>
       <c r="C25">
-        <v>252.43</v>
-      </c>
-      <c r="D25">
-        <f>324-C25</f>
         <v>71.569999999999993</v>
       </c>
       <c r="F25" t="s">
@@ -1211,7 +1180,7 @@
       </c>
       <c r="H25">
         <f>H17</f>
-        <v>71.5</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -1219,10 +1188,6 @@
         <v>91</v>
       </c>
       <c r="C26">
-        <v>217.75</v>
-      </c>
-      <c r="D26">
-        <f t="shared" ref="D26:D28" si="1">324-C26</f>
         <v>106.25</v>
       </c>
       <c r="F26" t="s">
@@ -1234,7 +1199,7 @@
       </c>
       <c r="H26">
         <f>H18</f>
-        <v>71.5</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -1242,10 +1207,6 @@
         <v>92</v>
       </c>
       <c r="C27">
-        <v>71.569999999999993</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="1"/>
         <v>252.43</v>
       </c>
       <c r="F27" t="s">
@@ -1257,7 +1218,7 @@
       </c>
       <c r="H27">
         <f>H28-C20</f>
-        <v>240.43</v>
+        <v>59.569999999999993</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -1265,10 +1226,6 @@
         <v>93</v>
       </c>
       <c r="C28">
-        <v>107.57</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="1"/>
         <v>216.43</v>
       </c>
       <c r="F28" t="s">
@@ -1280,7 +1237,7 @@
       </c>
       <c r="H28">
         <f>C25</f>
-        <v>252.43</v>
+        <v>71.569999999999993</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -1293,7 +1250,7 @@
       </c>
       <c r="H29">
         <f>H30+C20</f>
-        <v>83.57</v>
+        <v>264.43</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -1306,7 +1263,7 @@
       </c>
       <c r="H30">
         <f>C27</f>
-        <v>71.569999999999993</v>
+        <v>252.43</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -1319,7 +1276,7 @@
       </c>
       <c r="H31">
         <f>C26-C4</f>
-        <v>204</v>
+        <v>92.5</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -1332,7 +1289,7 @@
       </c>
       <c r="H32">
         <f>H31</f>
-        <v>204</v>
+        <v>92.5</v>
       </c>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.25">
@@ -1345,7 +1302,7 @@
       </c>
       <c r="H33">
         <f>C28+C4</f>
-        <v>121.32</v>
+        <v>230.18</v>
       </c>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.25">
@@ -1358,7 +1315,7 @@
       </c>
       <c r="H34">
         <f>H33</f>
-        <v>121.32</v>
+        <v>230.18</v>
       </c>
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.25">
@@ -1379,10 +1336,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B2C6CC-E6B0-438C-8DA4-A8209BB034F1}">
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,7 +1421,7 @@
       </c>
       <c r="E2" s="1">
         <f>RawPoints!H4</f>
-        <v>208.25</v>
+        <v>88.25</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -1475,7 +1432,7 @@
       </c>
       <c r="H2" s="1">
         <f>RawPoints!H15</f>
-        <v>222.75</v>
+        <v>69.25</v>
       </c>
       <c r="I2" s="1">
         <v>0</v>
@@ -1486,7 +1443,7 @@
       </c>
       <c r="K2" s="1">
         <f>RawPoints!H16</f>
-        <v>222.75</v>
+        <v>69.25</v>
       </c>
       <c r="L2" s="1">
         <v>0</v>
@@ -1508,7 +1465,7 @@
       </c>
       <c r="E3" s="1">
         <f>E2</f>
-        <v>208.25</v>
+        <v>88.25</v>
       </c>
       <c r="F3" s="1">
         <f>F2</f>
@@ -1520,7 +1477,7 @@
       </c>
       <c r="H3" s="1">
         <f>RawPoints!H17</f>
-        <v>71.5</v>
+        <v>189</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -1531,63 +1488,57 @@
       </c>
       <c r="K3" s="1">
         <f>H3</f>
-        <v>71.5</v>
+        <v>189</v>
       </c>
       <c r="L3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
         <f>D2</f>
         <v>16</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <f>RawPoints!H5</f>
-        <v>160.25</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" ref="G4:L4" si="0">G2</f>
+        <v>136.25</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <f>G2</f>
         <v>112</v>
       </c>
-      <c r="H4" s="3">
-        <f t="shared" si="0"/>
-        <v>222.75</v>
-      </c>
-      <c r="I4" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J4" s="3">
-        <f t="shared" si="0"/>
+      <c r="H4" s="1">
+        <f>H2</f>
+        <v>69.25</v>
+      </c>
+      <c r="I4" s="1">
+        <f>I2</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <f>J2</f>
         <v>124</v>
       </c>
-      <c r="K4" s="3">
-        <f t="shared" si="0"/>
-        <v>222.75</v>
-      </c>
-      <c r="L4" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
+      <c r="K4" s="1">
+        <f>K2</f>
+        <v>69.25</v>
+      </c>
+      <c r="L4" s="1">
+        <f>L2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1605,7 +1556,7 @@
       </c>
       <c r="E5" s="1">
         <f>E4</f>
-        <v>160.25</v>
+        <v>136.25</v>
       </c>
       <c r="F5" s="1">
         <f>F4</f>
@@ -1617,7 +1568,7 @@
       </c>
       <c r="H5" s="1">
         <f>H3</f>
-        <v>71.5</v>
+        <v>189</v>
       </c>
       <c r="I5" s="1">
         <f>I4</f>
@@ -1629,7 +1580,7 @@
       </c>
       <c r="K5" s="1">
         <f>K3</f>
-        <v>71.5</v>
+        <v>189</v>
       </c>
       <c r="L5" s="1">
         <f>L4</f>
@@ -1663,23 +1614,23 @@
         <v>112</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" ref="H6:L8" si="1">H4</f>
-        <v>222.75</v>
+        <f t="shared" ref="H6:L8" si="0">H4</f>
+        <v>69.25</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>124</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="1"/>
-        <v>222.75</v>
+        <f t="shared" si="0"/>
+        <v>69.25</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1706,27 +1657,27 @@
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" ref="G7:L7" si="2">G5</f>
+        <f t="shared" ref="G7:L7" si="1">G5</f>
         <v>112</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="2"/>
-        <v>71.5</v>
+        <f t="shared" si="1"/>
+        <v>189</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>124</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="2"/>
-        <v>71.5</v>
+        <f t="shared" si="1"/>
+        <v>189</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1746,7 +1697,7 @@
       </c>
       <c r="E8" s="1">
         <f>RawPoints!H3</f>
-        <v>307.75</v>
+        <v>43.75</v>
       </c>
       <c r="F8" s="1">
         <f>F7</f>
@@ -1757,23 +1708,23 @@
         <v>112</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="1"/>
-        <v>222.75</v>
+        <f t="shared" si="0"/>
+        <v>69.25</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>124</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="1"/>
-        <v>222.75</v>
+        <f t="shared" si="0"/>
+        <v>69.25</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1793,7 +1744,7 @@
       </c>
       <c r="E9" s="1">
         <f>E8</f>
-        <v>307.75</v>
+        <v>43.75</v>
       </c>
       <c r="F9" s="1">
         <f>F8</f>
@@ -1805,7 +1756,7 @@
       </c>
       <c r="H9" s="1">
         <f>RawPoints!H19</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
       <c r="I9" s="1">
         <v>75</v>
@@ -1816,7 +1767,7 @@
       </c>
       <c r="K9" s="1">
         <f>RawPoints!H20</f>
-        <v>222.75</v>
+        <v>69.25</v>
       </c>
       <c r="L9" s="1">
         <v>90</v>
@@ -1838,7 +1789,7 @@
       </c>
       <c r="E10" s="1">
         <f>RawPoints!H7</f>
-        <v>16.25</v>
+        <v>244.25</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -1849,7 +1800,7 @@
       </c>
       <c r="H10" s="1">
         <f>RawPoints!H21</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
       <c r="I10" s="1">
         <v>-75</v>
@@ -1860,7 +1811,7 @@
       </c>
       <c r="K10" s="1">
         <f>RawPoints!H22</f>
-        <v>101.25</v>
+        <v>218.75</v>
       </c>
       <c r="L10" s="1">
         <v>-90</v>
@@ -1882,7 +1833,7 @@
       </c>
       <c r="E11" s="1">
         <f>E2</f>
-        <v>208.25</v>
+        <v>88.25</v>
       </c>
       <c r="F11" s="1">
         <f>F10</f>
@@ -1893,7 +1844,7 @@
       </c>
       <c r="H11" s="1">
         <f>K11</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
       <c r="I11" s="1">
         <v>-25</v>
@@ -1904,7 +1855,7 @@
       </c>
       <c r="K11" s="1">
         <f>H9</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
       <c r="L11" s="1">
         <v>25</v>
@@ -1915,7 +1866,7 @@
       </c>
       <c r="N11" s="1">
         <f>K9</f>
-        <v>222.75</v>
+        <v>69.25</v>
       </c>
       <c r="O11" s="1">
         <v>90</v>
@@ -1947,7 +1898,7 @@
       </c>
       <c r="H12" s="1">
         <f>H10</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
       <c r="I12" s="1">
         <v>25</v>
@@ -1958,7 +1909,7 @@
       </c>
       <c r="K12" s="1">
         <f>H10</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
       <c r="L12" s="1">
         <v>-25</v>
@@ -1969,7 +1920,7 @@
       </c>
       <c r="N12" s="1">
         <f>K10</f>
-        <v>101.25</v>
+        <v>218.75</v>
       </c>
       <c r="O12" s="1">
         <v>-90</v>
@@ -1991,7 +1942,7 @@
       </c>
       <c r="E13" s="1">
         <f>E8</f>
-        <v>307.75</v>
+        <v>43.75</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -2002,7 +1953,7 @@
       </c>
       <c r="H13" s="1">
         <f>H11</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
       <c r="I13" s="1">
         <v>-25</v>
@@ -2013,7 +1964,7 @@
       </c>
       <c r="K13" s="1">
         <f>H13</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
       <c r="L13" s="1">
         <v>25</v>
@@ -2024,7 +1975,7 @@
       </c>
       <c r="N13" s="1">
         <f>RawPoints!H23</f>
-        <v>222.75</v>
+        <v>69.25</v>
       </c>
       <c r="O13" s="1">
         <v>125</v>
@@ -2035,7 +1986,7 @@
       </c>
       <c r="Q13" s="1">
         <f>RawPoints!H24</f>
-        <v>222.75</v>
+        <v>69.25</v>
       </c>
       <c r="R13" s="1">
         <v>180</v>
@@ -2057,7 +2008,7 @@
       </c>
       <c r="E14" s="1">
         <f>E2</f>
-        <v>208.25</v>
+        <v>88.25</v>
       </c>
       <c r="F14" s="1">
         <f>F13</f>
@@ -2069,18 +2020,18 @@
       </c>
       <c r="H14" s="1">
         <f>H13</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
       <c r="I14" s="1">
         <v>-25</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" ref="J14:J16" si="3">M14</f>
+        <f t="shared" ref="J14:J16" si="2">M14</f>
         <v>208</v>
       </c>
       <c r="K14" s="1">
         <f>H14</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
       <c r="L14" s="1">
         <v>25</v>
@@ -2090,20 +2041,20 @@
         <v>208</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" ref="N14:Q14" si="4">N13</f>
-        <v>222.75</v>
+        <f t="shared" ref="N14:R14" si="3">N13</f>
+        <v>69.25</v>
       </c>
       <c r="O14" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>125</v>
       </c>
       <c r="P14" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>196</v>
       </c>
       <c r="Q14" s="1">
-        <f t="shared" si="4"/>
-        <v>222.75</v>
+        <f t="shared" si="3"/>
+        <v>69.25</v>
       </c>
       <c r="R14" s="1">
         <v>180</v>
@@ -2135,18 +2086,18 @@
       </c>
       <c r="H15" s="1">
         <f>H12</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
       <c r="I15" s="1">
         <v>25</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>208</v>
       </c>
       <c r="K15" s="1">
         <f>H15</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
       <c r="L15" s="1">
         <v>-25</v>
@@ -2157,7 +2108,7 @@
       </c>
       <c r="N15" s="1">
         <f>RawPoints!H25</f>
-        <v>71.5</v>
+        <v>189</v>
       </c>
       <c r="O15" s="1">
         <v>-125</v>
@@ -2168,7 +2119,7 @@
       </c>
       <c r="Q15" s="1">
         <f>N15</f>
-        <v>71.5</v>
+        <v>189</v>
       </c>
       <c r="R15" s="1">
         <v>180</v>
@@ -2190,7 +2141,7 @@
       </c>
       <c r="E16" s="1">
         <f>E10</f>
-        <v>16.25</v>
+        <v>244.25</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -2200,18 +2151,18 @@
       </c>
       <c r="H16" s="1">
         <f>H12</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
       <c r="I16" s="1">
         <v>25</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>208</v>
       </c>
       <c r="K16" s="1">
         <f>H16</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
       <c r="L16" s="1">
         <v>-25</v>
@@ -2222,7 +2173,7 @@
       </c>
       <c r="N16" s="1">
         <f>N15</f>
-        <v>71.5</v>
+        <v>189</v>
       </c>
       <c r="O16" s="1">
         <v>-125</v>
@@ -2233,7 +2184,7 @@
       </c>
       <c r="Q16" s="1">
         <f>Q15</f>
-        <v>71.5</v>
+        <v>189</v>
       </c>
       <c r="R16" s="1">
         <v>180</v>
@@ -2255,7 +2206,7 @@
       </c>
       <c r="E17" s="1">
         <f>E16</f>
-        <v>16.25</v>
+        <v>244.25</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -2266,7 +2217,7 @@
       </c>
       <c r="H17" s="1">
         <f>H7</f>
-        <v>71.5</v>
+        <v>189</v>
       </c>
       <c r="I17" s="1">
         <f>I8</f>
@@ -2278,7 +2229,7 @@
       </c>
       <c r="K17" s="1">
         <f>K7</f>
-        <v>71.5</v>
+        <v>189</v>
       </c>
       <c r="L17" s="1">
         <f>L8</f>
@@ -2301,7 +2252,7 @@
       </c>
       <c r="E18" s="1">
         <f>E8</f>
-        <v>307.75</v>
+        <v>43.75</v>
       </c>
       <c r="F18" s="1">
         <f>F17</f>
@@ -2313,7 +2264,7 @@
       </c>
       <c r="H18" s="1">
         <f>H14</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
       <c r="I18" s="1">
         <v>-25</v>
@@ -2324,7 +2275,7 @@
       </c>
       <c r="K18" s="1">
         <f>RawPoints!H27</f>
-        <v>240.43</v>
+        <v>59.569999999999993</v>
       </c>
       <c r="L18" s="1">
         <v>25</v>
@@ -2335,7 +2286,7 @@
       </c>
       <c r="N18" s="1">
         <f>RawPoints!H28</f>
-        <v>252.43</v>
+        <v>71.569999999999993</v>
       </c>
       <c r="O18" s="1">
         <v>90</v>
@@ -2352,24 +2303,24 @@
         <v>5</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" ref="D19:D29" si="5">D18</f>
+        <f t="shared" ref="D19:D29" si="4">D18</f>
         <v>16</v>
       </c>
       <c r="E19" s="1">
         <f>E18</f>
-        <v>307.75</v>
+        <v>43.75</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" ref="F19:F25" si="6">F18</f>
+        <f t="shared" ref="F19:F25" si="5">F18</f>
         <v>0</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" ref="G19:G25" si="7">G16</f>
+        <f t="shared" ref="G19:G25" si="6">G16</f>
         <v>140</v>
       </c>
       <c r="H19" s="1">
         <f>H18</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
       <c r="I19" s="1">
         <f>I18</f>
@@ -2381,7 +2332,7 @@
       </c>
       <c r="K19" s="1">
         <f>H19</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
       <c r="L19" s="1">
         <v>25</v>
@@ -2392,7 +2343,7 @@
       </c>
       <c r="N19" s="1">
         <f>RawPoints!H31</f>
-        <v>204</v>
+        <v>92.5</v>
       </c>
       <c r="O19" s="1">
         <v>45</v>
@@ -2403,7 +2354,7 @@
       </c>
       <c r="Q19" s="1">
         <f>N19</f>
-        <v>204</v>
+        <v>92.5</v>
       </c>
       <c r="R19" s="1">
         <v>0</v>
@@ -2420,15 +2371,15 @@
         <v>4</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="E20" s="1">
         <f>E2</f>
-        <v>208.25</v>
+        <v>88.25</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G20" s="1">
@@ -2437,7 +2388,7 @@
       </c>
       <c r="H20" s="1">
         <f>H19</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
       <c r="I20" s="1">
         <v>25</v>
@@ -2448,21 +2399,21 @@
       </c>
       <c r="K20" s="1">
         <f>K18</f>
-        <v>240.43</v>
+        <v>59.569999999999993</v>
       </c>
       <c r="L20" s="1">
         <v>-25</v>
       </c>
       <c r="M20" s="1">
-        <f t="shared" ref="M20:O21" si="8">M18</f>
+        <f>M18</f>
         <v>324</v>
       </c>
       <c r="N20" s="1">
-        <f t="shared" si="8"/>
-        <v>252.43</v>
+        <f>N18</f>
+        <v>71.569999999999993</v>
       </c>
       <c r="O20" s="1">
-        <f t="shared" si="8"/>
+        <f>O18</f>
         <v>90</v>
       </c>
     </row>
@@ -2477,24 +2428,24 @@
         <v>5</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="E21" s="1">
         <f>E20</f>
-        <v>208.25</v>
+        <v>88.25</v>
       </c>
       <c r="F21" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="1">
-        <f t="shared" si="7"/>
         <v>140</v>
       </c>
       <c r="H21" s="1">
         <f>H20</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
       <c r="I21" s="1">
         <f>I20</f>
@@ -2506,21 +2457,21 @@
       </c>
       <c r="K21" s="1">
         <f>H21</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
       <c r="L21" s="1">
         <v>-25</v>
       </c>
       <c r="M21" s="1">
-        <f t="shared" si="8"/>
+        <f>M19</f>
         <v>288</v>
       </c>
       <c r="N21" s="1">
-        <f t="shared" si="8"/>
-        <v>204</v>
+        <f>N19</f>
+        <v>92.5</v>
       </c>
       <c r="O21" s="1">
-        <f t="shared" si="8"/>
+        <f>O19</f>
         <v>45</v>
       </c>
       <c r="P21" s="1">
@@ -2529,7 +2480,7 @@
       </c>
       <c r="Q21" s="1">
         <f>Q19</f>
-        <v>204</v>
+        <v>92.5</v>
       </c>
       <c r="R21" s="1">
         <f>R19</f>
@@ -2547,7 +2498,7 @@
         <v>4</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="E22" s="1">
@@ -2555,16 +2506,16 @@
         <v>182.25</v>
       </c>
       <c r="F22" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="1">
-        <f t="shared" si="7"/>
         <v>140</v>
       </c>
       <c r="H22" s="1">
         <f>H15</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
       <c r="I22" s="1">
         <v>25</v>
@@ -2575,7 +2526,7 @@
       </c>
       <c r="K22" s="1">
         <f>RawPoints!H29</f>
-        <v>83.57</v>
+        <v>264.43</v>
       </c>
       <c r="L22" s="1">
         <v>-25</v>
@@ -2586,7 +2537,7 @@
       </c>
       <c r="N22" s="1">
         <f>RawPoints!H30</f>
-        <v>71.569999999999993</v>
+        <v>252.43</v>
       </c>
       <c r="O22" s="1">
         <v>-90</v>
@@ -2603,7 +2554,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="E23" s="1">
@@ -2611,7 +2562,7 @@
         <v>182.25</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G23" s="1">
@@ -2620,7 +2571,7 @@
       </c>
       <c r="H23" s="1">
         <f>H22</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
       <c r="I23" s="1">
         <f>I22</f>
@@ -2632,7 +2583,7 @@
       </c>
       <c r="K23" s="1">
         <f>H23</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
       <c r="L23" s="1">
         <v>-25</v>
@@ -2643,7 +2594,7 @@
       </c>
       <c r="N23" s="1">
         <f>RawPoints!H33</f>
-        <v>121.32</v>
+        <v>230.18</v>
       </c>
       <c r="O23" s="1">
         <v>-90</v>
@@ -2654,7 +2605,7 @@
       </c>
       <c r="Q23" s="1">
         <f>N23</f>
-        <v>121.32</v>
+        <v>230.18</v>
       </c>
       <c r="R23" s="1">
         <v>0</v>
@@ -2671,24 +2622,24 @@
         <v>4</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="E24" s="1">
         <f>E16</f>
-        <v>16.25</v>
+        <v>244.25</v>
       </c>
       <c r="F24" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="1">
-        <f t="shared" si="7"/>
         <v>140</v>
       </c>
       <c r="H24" s="1">
         <f>H23</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
       <c r="I24" s="1">
         <f>I23</f>
@@ -2700,7 +2651,7 @@
       </c>
       <c r="K24" s="1">
         <f>K22</f>
-        <v>83.57</v>
+        <v>264.43</v>
       </c>
       <c r="L24" s="1">
         <v>-75</v>
@@ -2711,7 +2662,7 @@
       </c>
       <c r="N24" s="1">
         <f>N22</f>
-        <v>71.569999999999993</v>
+        <v>252.43</v>
       </c>
       <c r="O24" s="1">
         <v>-90</v>
@@ -2728,24 +2679,24 @@
         <v>5</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="E25" s="1">
         <f>E24</f>
-        <v>16.25</v>
+        <v>244.25</v>
       </c>
       <c r="F25" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="1">
-        <f t="shared" si="7"/>
         <v>140</v>
       </c>
       <c r="H25" s="1">
         <f>H24</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
       <c r="I25" s="1">
         <f>I24</f>
@@ -2757,7 +2708,7 @@
       </c>
       <c r="K25" s="1">
         <f>H25</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
       <c r="L25" s="1">
         <v>-75</v>
@@ -2768,7 +2719,7 @@
       </c>
       <c r="N25" s="1">
         <f>N23</f>
-        <v>121.32</v>
+        <v>230.18</v>
       </c>
       <c r="O25" s="1">
         <f>O23</f>
@@ -2780,7 +2731,7 @@
       </c>
       <c r="Q25" s="1">
         <f>Q23</f>
-        <v>121.32</v>
+        <v>230.18</v>
       </c>
       <c r="R25" s="1">
         <f>R23</f>
@@ -2798,12 +2749,12 @@
         <v>5</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="E26" s="1">
         <f>E18</f>
-        <v>307.75</v>
+        <v>43.75</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -2814,7 +2765,7 @@
       </c>
       <c r="H26" s="1">
         <f>H20</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
       <c r="I26" s="1">
         <v>-25</v>
@@ -2825,7 +2776,7 @@
       </c>
       <c r="K26" s="1">
         <f>H26</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
       <c r="L26" s="1">
         <v>25</v>
@@ -2836,7 +2787,7 @@
       </c>
       <c r="N26" s="1">
         <f>N23</f>
-        <v>121.32</v>
+        <v>230.18</v>
       </c>
       <c r="O26" s="1">
         <v>-25</v>
@@ -2847,7 +2798,7 @@
       </c>
       <c r="Q26" s="1">
         <f>Q25</f>
-        <v>121.32</v>
+        <v>230.18</v>
       </c>
       <c r="R26" s="1">
         <f>R25</f>
@@ -2865,23 +2816,23 @@
         <v>5</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="E27" s="1">
         <f>E26</f>
-        <v>307.75</v>
+        <v>43.75</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" ref="G27:G29" si="9">G26</f>
+        <f t="shared" ref="G27:G29" si="7">G26</f>
         <v>140</v>
       </c>
       <c r="H27" s="1">
         <f>H26</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
       <c r="I27" s="1">
         <v>-25</v>
@@ -2892,7 +2843,7 @@
       </c>
       <c r="K27" s="1">
         <f>H27</f>
-        <v>210.75</v>
+        <v>57.25</v>
       </c>
       <c r="L27" s="1">
         <v>25</v>
@@ -2903,7 +2854,7 @@
       </c>
       <c r="N27" s="1">
         <f>N26</f>
-        <v>121.32</v>
+        <v>230.18</v>
       </c>
       <c r="O27" s="1">
         <v>-25</v>
@@ -2914,7 +2865,7 @@
       </c>
       <c r="Q27" s="1">
         <f>Q26</f>
-        <v>121.32</v>
+        <v>230.18</v>
       </c>
       <c r="R27" s="1">
         <f>R26</f>
@@ -2932,34 +2883,34 @@
         <v>5</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="E28" s="1">
         <f>E24</f>
-        <v>16.25</v>
+        <v>244.25</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
       </c>
       <c r="G28" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>140</v>
       </c>
       <c r="H28" s="1">
         <f>H25</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
       <c r="I28" s="1">
         <v>25</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" ref="J28:J29" si="10">J27</f>
+        <f t="shared" ref="J28:J29" si="8">J27</f>
         <v>228.75</v>
       </c>
       <c r="K28" s="1">
         <f>K23</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
       <c r="L28" s="1">
         <v>-25</v>
@@ -2970,7 +2921,7 @@
       </c>
       <c r="N28" s="1">
         <f>N21</f>
-        <v>204</v>
+        <v>92.5</v>
       </c>
       <c r="O28" s="1">
         <v>25</v>
@@ -2981,7 +2932,7 @@
       </c>
       <c r="Q28" s="1">
         <f>Q21</f>
-        <v>204</v>
+        <v>92.5</v>
       </c>
       <c r="R28" s="1">
         <v>0</v>
@@ -2998,35 +2949,35 @@
         <v>5</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="E29" s="1">
         <f>E25</f>
-        <v>16.25</v>
+        <v>244.25</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
       </c>
       <c r="G29" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>140</v>
       </c>
       <c r="H29" s="1">
         <f>H28</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
       <c r="I29" s="1">
         <f>I25</f>
         <v>25</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>228.75</v>
       </c>
       <c r="K29" s="1">
         <f>H29</f>
-        <v>113.25</v>
+        <v>230.75</v>
       </c>
       <c r="L29" s="1">
         <f>L28</f>
@@ -3038,7 +2989,7 @@
       </c>
       <c r="N29" s="1">
         <f>N28</f>
-        <v>204</v>
+        <v>92.5</v>
       </c>
       <c r="O29" s="1">
         <v>25</v>
@@ -3049,7 +3000,7 @@
       </c>
       <c r="Q29" s="1">
         <f>N29</f>
-        <v>204</v>
+        <v>92.5</v>
       </c>
       <c r="R29" s="1">
         <v>0</v>
@@ -3086,10 +3037,10 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -3104,41 +3055,12 @@
         <v>0</v>
       </c>
       <c r="G31" s="1">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="H31" s="1">
         <v>0</v>
       </c>
       <c r="I31" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>114</v>
-      </c>
-      <c r="B32" t="s">
-        <v>113</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
-      <c r="D32" s="1">
-        <v>0</v>
-      </c>
-      <c r="E32" s="1">
-        <v>0</v>
-      </c>
-      <c r="F32" s="1">
-        <v>0</v>
-      </c>
-      <c r="G32" s="1">
-        <v>120</v>
-      </c>
-      <c r="H32" s="1">
-        <v>0</v>
-      </c>
-      <c r="I32" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "Check in auto and fix to the user controls""
This reverts commit 4fff0788ebed72c1af9f0a5e1b555acedf22e77f.
</commit_message>
<xml_diff>
--- a/Paths.xlsx
+++ b/Paths.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19740" windowHeight="5910" xr2:uid="{84364B8A-653F-400C-BF42-269DA731DB7B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19740" windowHeight="5910" activeTab="1" xr2:uid="{84364B8A-653F-400C-BF42-269DA731DB7B}"/>
   </bookViews>
   <sheets>
     <sheet name="RawPoints" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="117">
   <si>
     <t>FieldXRedWall</t>
   </si>
@@ -370,6 +370,12 @@
   </si>
   <si>
     <t>Bad</t>
+  </si>
+  <si>
+    <t>Move8</t>
+  </si>
+  <si>
+    <t>Move eight feet</t>
   </si>
 </sst>
 </file>
@@ -385,12 +391,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -405,9 +417,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -726,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDDAE613-BBFC-4F5C-AD8E-7A070BBCC1B5}">
   <dimension ref="B1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection sqref="A1:H35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +787,7 @@
       </c>
       <c r="H3">
         <f>C10+C4</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -791,7 +807,7 @@
       </c>
       <c r="H4">
         <f>C18-C4</f>
-        <v>88.25</v>
+        <v>208.25</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -811,7 +827,7 @@
       </c>
       <c r="H5">
         <f>C19-C4</f>
-        <v>136.25</v>
+        <v>160.25</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -850,7 +866,7 @@
       </c>
       <c r="H7">
         <f>C11-C4</f>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -858,7 +874,7 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>324</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -866,8 +882,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <f>24*12</f>
-        <v>288</v>
+        <v>0</v>
       </c>
       <c r="F9" t="s">
         <v>35</v>
@@ -878,7 +893,7 @@
       </c>
       <c r="H9">
         <f>H3</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -886,8 +901,8 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <f>C8+30</f>
-        <v>30</v>
+        <f>C8-30</f>
+        <v>294</v>
       </c>
       <c r="F10" t="s">
         <v>39</v>
@@ -898,7 +913,7 @@
       </c>
       <c r="H10">
         <f t="shared" ref="H10:H13" si="0">H4</f>
-        <v>88.25</v>
+        <v>208.25</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -906,8 +921,8 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <f>C9-30</f>
-        <v>258</v>
+        <f>C9+30</f>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
         <v>36</v>
@@ -918,7 +933,7 @@
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>136.25</v>
+        <v>160.25</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -958,7 +973,7 @@
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -987,7 +1002,7 @@
       </c>
       <c r="H15">
         <f>C21-C5</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -1007,7 +1022,7 @@
       </c>
       <c r="H16">
         <f>H15</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -1027,7 +1042,7 @@
       </c>
       <c r="H17">
         <f>C22-C4</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -1035,6 +1050,10 @@
         <v>19</v>
       </c>
       <c r="C18">
+        <v>222</v>
+      </c>
+      <c r="D18">
+        <f>324-C18</f>
         <v>102</v>
       </c>
       <c r="F18" t="s">
@@ -1046,7 +1065,7 @@
       </c>
       <c r="H18">
         <f>H17</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1054,6 +1073,10 @@
         <v>20</v>
       </c>
       <c r="C19">
+        <v>174</v>
+      </c>
+      <c r="D19">
+        <f>324-C19</f>
         <v>150</v>
       </c>
       <c r="F19" t="s">
@@ -1065,7 +1088,7 @@
       </c>
       <c r="H19">
         <f>H20-C20</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1084,7 +1107,7 @@
       </c>
       <c r="H20">
         <f>C21-C5</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1092,6 +1115,10 @@
         <v>22</v>
       </c>
       <c r="C21">
+        <v>238.75</v>
+      </c>
+      <c r="D21">
+        <f>324-C21</f>
         <v>85.25</v>
       </c>
       <c r="F21" t="s">
@@ -1103,7 +1130,7 @@
       </c>
       <c r="H21">
         <f>H22+C20</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -1111,8 +1138,8 @@
         <v>23</v>
       </c>
       <c r="C22">
-        <f>C9-C21</f>
-        <v>202.75</v>
+        <f>C8-C21</f>
+        <v>85.25</v>
       </c>
       <c r="F22" t="s">
         <v>34</v>
@@ -1123,7 +1150,7 @@
       </c>
       <c r="H22">
         <f>C22+C5</f>
-        <v>218.75</v>
+        <v>101.25</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -1142,7 +1169,7 @@
       </c>
       <c r="H23">
         <f>H15</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1161,7 +1188,7 @@
       </c>
       <c r="H24">
         <f>H16</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1169,6 +1196,10 @@
         <v>90</v>
       </c>
       <c r="C25">
+        <v>252.43</v>
+      </c>
+      <c r="D25">
+        <f>324-C25</f>
         <v>71.569999999999993</v>
       </c>
       <c r="F25" t="s">
@@ -1180,7 +1211,7 @@
       </c>
       <c r="H25">
         <f>H17</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -1188,6 +1219,10 @@
         <v>91</v>
       </c>
       <c r="C26">
+        <v>217.75</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ref="D26:D28" si="1">324-C26</f>
         <v>106.25</v>
       </c>
       <c r="F26" t="s">
@@ -1199,7 +1234,7 @@
       </c>
       <c r="H26">
         <f>H18</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -1207,6 +1242,10 @@
         <v>92</v>
       </c>
       <c r="C27">
+        <v>71.569999999999993</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
         <v>252.43</v>
       </c>
       <c r="F27" t="s">
@@ -1218,7 +1257,7 @@
       </c>
       <c r="H27">
         <f>H28-C20</f>
-        <v>59.569999999999993</v>
+        <v>240.43</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -1226,6 +1265,10 @@
         <v>93</v>
       </c>
       <c r="C28">
+        <v>107.57</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
         <v>216.43</v>
       </c>
       <c r="F28" t="s">
@@ -1237,7 +1280,7 @@
       </c>
       <c r="H28">
         <f>C25</f>
-        <v>71.569999999999993</v>
+        <v>252.43</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -1250,7 +1293,7 @@
       </c>
       <c r="H29">
         <f>H30+C20</f>
-        <v>264.43</v>
+        <v>83.57</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -1263,7 +1306,7 @@
       </c>
       <c r="H30">
         <f>C27</f>
-        <v>252.43</v>
+        <v>71.569999999999993</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -1276,7 +1319,7 @@
       </c>
       <c r="H31">
         <f>C26-C4</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -1289,7 +1332,7 @@
       </c>
       <c r="H32">
         <f>H31</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.25">
@@ -1302,7 +1345,7 @@
       </c>
       <c r="H33">
         <f>C28+C4</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.25">
@@ -1315,7 +1358,7 @@
       </c>
       <c r="H34">
         <f>H33</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.25">
@@ -1336,10 +1379,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B2C6CC-E6B0-438C-8DA4-A8209BB034F1}">
-  <dimension ref="A1:R31"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,7 +1464,7 @@
       </c>
       <c r="E2" s="1">
         <f>RawPoints!H4</f>
-        <v>88.25</v>
+        <v>208.25</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -1432,7 +1475,7 @@
       </c>
       <c r="H2" s="1">
         <f>RawPoints!H15</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
       <c r="I2" s="1">
         <v>0</v>
@@ -1443,7 +1486,7 @@
       </c>
       <c r="K2" s="1">
         <f>RawPoints!H16</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
       <c r="L2" s="1">
         <v>0</v>
@@ -1465,7 +1508,7 @@
       </c>
       <c r="E3" s="1">
         <f>E2</f>
-        <v>88.25</v>
+        <v>208.25</v>
       </c>
       <c r="F3" s="1">
         <f>F2</f>
@@ -1477,7 +1520,7 @@
       </c>
       <c r="H3" s="1">
         <f>RawPoints!H17</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -1488,57 +1531,63 @@
       </c>
       <c r="K3" s="1">
         <f>H3</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="L3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
         <f>D2</f>
         <v>16</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
         <f>RawPoints!H5</f>
-        <v>136.25</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <f>G2</f>
+        <v>160.25</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" ref="G4:L4" si="0">G2</f>
         <v>112</v>
       </c>
-      <c r="H4" s="1">
-        <f>H2</f>
-        <v>69.25</v>
-      </c>
-      <c r="I4" s="1">
-        <f>I2</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <f>J2</f>
+      <c r="H4" s="3">
+        <f t="shared" si="0"/>
+        <v>222.75</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="0"/>
         <v>124</v>
       </c>
-      <c r="K4" s="1">
-        <f>K2</f>
-        <v>69.25</v>
-      </c>
-      <c r="L4" s="1">
-        <f>L2</f>
-        <v>0</v>
-      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="0"/>
+        <v>222.75</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1556,7 +1605,7 @@
       </c>
       <c r="E5" s="1">
         <f>E4</f>
-        <v>136.25</v>
+        <v>160.25</v>
       </c>
       <c r="F5" s="1">
         <f>F4</f>
@@ -1568,7 +1617,7 @@
       </c>
       <c r="H5" s="1">
         <f>H3</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="I5" s="1">
         <f>I4</f>
@@ -1580,7 +1629,7 @@
       </c>
       <c r="K5" s="1">
         <f>K3</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="L5" s="1">
         <f>L4</f>
@@ -1614,23 +1663,23 @@
         <v>112</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" ref="H6:L8" si="0">H4</f>
-        <v>69.25</v>
+        <f t="shared" ref="H6:L8" si="1">H4</f>
+        <v>222.75</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>124</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="0"/>
-        <v>69.25</v>
+        <f t="shared" si="1"/>
+        <v>222.75</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1657,27 +1706,27 @@
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" ref="G7:L7" si="1">G5</f>
+        <f t="shared" ref="G7:L7" si="2">G5</f>
         <v>112</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="1"/>
-        <v>189</v>
+        <f t="shared" si="2"/>
+        <v>71.5</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>124</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="1"/>
-        <v>189</v>
+        <f t="shared" si="2"/>
+        <v>71.5</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1697,7 +1746,7 @@
       </c>
       <c r="E8" s="1">
         <f>RawPoints!H3</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
       <c r="F8" s="1">
         <f>F7</f>
@@ -1708,23 +1757,23 @@
         <v>112</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="0"/>
-        <v>69.25</v>
+        <f t="shared" si="1"/>
+        <v>222.75</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>124</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="0"/>
-        <v>69.25</v>
+        <f t="shared" si="1"/>
+        <v>222.75</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1744,7 +1793,7 @@
       </c>
       <c r="E9" s="1">
         <f>E8</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
       <c r="F9" s="1">
         <f>F8</f>
@@ -1756,7 +1805,7 @@
       </c>
       <c r="H9" s="1">
         <f>RawPoints!H19</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I9" s="1">
         <v>75</v>
@@ -1767,7 +1816,7 @@
       </c>
       <c r="K9" s="1">
         <f>RawPoints!H20</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
       <c r="L9" s="1">
         <v>90</v>
@@ -1789,7 +1838,7 @@
       </c>
       <c r="E10" s="1">
         <f>RawPoints!H7</f>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -1800,7 +1849,7 @@
       </c>
       <c r="H10" s="1">
         <f>RawPoints!H21</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I10" s="1">
         <v>-75</v>
@@ -1811,7 +1860,7 @@
       </c>
       <c r="K10" s="1">
         <f>RawPoints!H22</f>
-        <v>218.75</v>
+        <v>101.25</v>
       </c>
       <c r="L10" s="1">
         <v>-90</v>
@@ -1833,7 +1882,7 @@
       </c>
       <c r="E11" s="1">
         <f>E2</f>
-        <v>88.25</v>
+        <v>208.25</v>
       </c>
       <c r="F11" s="1">
         <f>F10</f>
@@ -1844,7 +1893,7 @@
       </c>
       <c r="H11" s="1">
         <f>K11</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I11" s="1">
         <v>-25</v>
@@ -1855,7 +1904,7 @@
       </c>
       <c r="K11" s="1">
         <f>H9</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="L11" s="1">
         <v>25</v>
@@ -1866,7 +1915,7 @@
       </c>
       <c r="N11" s="1">
         <f>K9</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
       <c r="O11" s="1">
         <v>90</v>
@@ -1898,7 +1947,7 @@
       </c>
       <c r="H12" s="1">
         <f>H10</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I12" s="1">
         <v>25</v>
@@ -1909,7 +1958,7 @@
       </c>
       <c r="K12" s="1">
         <f>H10</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="L12" s="1">
         <v>-25</v>
@@ -1920,7 +1969,7 @@
       </c>
       <c r="N12" s="1">
         <f>K10</f>
-        <v>218.75</v>
+        <v>101.25</v>
       </c>
       <c r="O12" s="1">
         <v>-90</v>
@@ -1942,7 +1991,7 @@
       </c>
       <c r="E13" s="1">
         <f>E8</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -1953,7 +2002,7 @@
       </c>
       <c r="H13" s="1">
         <f>H11</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I13" s="1">
         <v>-25</v>
@@ -1964,7 +2013,7 @@
       </c>
       <c r="K13" s="1">
         <f>H13</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="L13" s="1">
         <v>25</v>
@@ -1975,7 +2024,7 @@
       </c>
       <c r="N13" s="1">
         <f>RawPoints!H23</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
       <c r="O13" s="1">
         <v>125</v>
@@ -1986,7 +2035,7 @@
       </c>
       <c r="Q13" s="1">
         <f>RawPoints!H24</f>
-        <v>69.25</v>
+        <v>222.75</v>
       </c>
       <c r="R13" s="1">
         <v>180</v>
@@ -2008,7 +2057,7 @@
       </c>
       <c r="E14" s="1">
         <f>E2</f>
-        <v>88.25</v>
+        <v>208.25</v>
       </c>
       <c r="F14" s="1">
         <f>F13</f>
@@ -2020,18 +2069,18 @@
       </c>
       <c r="H14" s="1">
         <f>H13</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I14" s="1">
         <v>-25</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" ref="J14:J16" si="2">M14</f>
+        <f t="shared" ref="J14:J16" si="3">M14</f>
         <v>208</v>
       </c>
       <c r="K14" s="1">
         <f>H14</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="L14" s="1">
         <v>25</v>
@@ -2041,20 +2090,20 @@
         <v>208</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" ref="N14:R14" si="3">N13</f>
-        <v>69.25</v>
+        <f t="shared" ref="N14:Q14" si="4">N13</f>
+        <v>222.75</v>
       </c>
       <c r="O14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>125</v>
       </c>
       <c r="P14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>196</v>
       </c>
       <c r="Q14" s="1">
-        <f t="shared" si="3"/>
-        <v>69.25</v>
+        <f t="shared" si="4"/>
+        <v>222.75</v>
       </c>
       <c r="R14" s="1">
         <v>180</v>
@@ -2086,18 +2135,18 @@
       </c>
       <c r="H15" s="1">
         <f>H12</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I15" s="1">
         <v>25</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>208</v>
       </c>
       <c r="K15" s="1">
         <f>H15</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="L15" s="1">
         <v>-25</v>
@@ -2108,7 +2157,7 @@
       </c>
       <c r="N15" s="1">
         <f>RawPoints!H25</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="O15" s="1">
         <v>-125</v>
@@ -2119,7 +2168,7 @@
       </c>
       <c r="Q15" s="1">
         <f>N15</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="R15" s="1">
         <v>180</v>
@@ -2141,7 +2190,7 @@
       </c>
       <c r="E16" s="1">
         <f>E10</f>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -2151,18 +2200,18 @@
       </c>
       <c r="H16" s="1">
         <f>H12</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I16" s="1">
         <v>25</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>208</v>
       </c>
       <c r="K16" s="1">
         <f>H16</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="L16" s="1">
         <v>-25</v>
@@ -2173,7 +2222,7 @@
       </c>
       <c r="N16" s="1">
         <f>N15</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="O16" s="1">
         <v>-125</v>
@@ -2184,7 +2233,7 @@
       </c>
       <c r="Q16" s="1">
         <f>Q15</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="R16" s="1">
         <v>180</v>
@@ -2206,7 +2255,7 @@
       </c>
       <c r="E17" s="1">
         <f>E16</f>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -2217,7 +2266,7 @@
       </c>
       <c r="H17" s="1">
         <f>H7</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="I17" s="1">
         <f>I8</f>
@@ -2229,7 +2278,7 @@
       </c>
       <c r="K17" s="1">
         <f>K7</f>
-        <v>189</v>
+        <v>71.5</v>
       </c>
       <c r="L17" s="1">
         <f>L8</f>
@@ -2252,7 +2301,7 @@
       </c>
       <c r="E18" s="1">
         <f>E8</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
       <c r="F18" s="1">
         <f>F17</f>
@@ -2264,7 +2313,7 @@
       </c>
       <c r="H18" s="1">
         <f>H14</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I18" s="1">
         <v>-25</v>
@@ -2275,7 +2324,7 @@
       </c>
       <c r="K18" s="1">
         <f>RawPoints!H27</f>
-        <v>59.569999999999993</v>
+        <v>240.43</v>
       </c>
       <c r="L18" s="1">
         <v>25</v>
@@ -2286,7 +2335,7 @@
       </c>
       <c r="N18" s="1">
         <f>RawPoints!H28</f>
-        <v>71.569999999999993</v>
+        <v>252.43</v>
       </c>
       <c r="O18" s="1">
         <v>90</v>
@@ -2303,24 +2352,24 @@
         <v>5</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" ref="D19:D29" si="4">D18</f>
+        <f t="shared" ref="D19:D29" si="5">D18</f>
         <v>16</v>
       </c>
       <c r="E19" s="1">
         <f>E18</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" ref="F19:F25" si="5">F18</f>
+        <f t="shared" ref="F19:F25" si="6">F18</f>
         <v>0</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" ref="G19:G25" si="6">G16</f>
+        <f t="shared" ref="G19:G25" si="7">G16</f>
         <v>140</v>
       </c>
       <c r="H19" s="1">
         <f>H18</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I19" s="1">
         <f>I18</f>
@@ -2332,7 +2381,7 @@
       </c>
       <c r="K19" s="1">
         <f>H19</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="L19" s="1">
         <v>25</v>
@@ -2343,7 +2392,7 @@
       </c>
       <c r="N19" s="1">
         <f>RawPoints!H31</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
       <c r="O19" s="1">
         <v>45</v>
@@ -2354,7 +2403,7 @@
       </c>
       <c r="Q19" s="1">
         <f>N19</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
       <c r="R19" s="1">
         <v>0</v>
@@ -2371,15 +2420,15 @@
         <v>4</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E20" s="1">
         <f>E2</f>
-        <v>88.25</v>
+        <v>208.25</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G20" s="1">
@@ -2388,7 +2437,7 @@
       </c>
       <c r="H20" s="1">
         <f>H19</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I20" s="1">
         <v>25</v>
@@ -2399,21 +2448,21 @@
       </c>
       <c r="K20" s="1">
         <f>K18</f>
-        <v>59.569999999999993</v>
+        <v>240.43</v>
       </c>
       <c r="L20" s="1">
         <v>-25</v>
       </c>
       <c r="M20" s="1">
-        <f>M18</f>
+        <f t="shared" ref="M20:O21" si="8">M18</f>
         <v>324</v>
       </c>
       <c r="N20" s="1">
-        <f>N18</f>
-        <v>71.569999999999993</v>
+        <f t="shared" si="8"/>
+        <v>252.43</v>
       </c>
       <c r="O20" s="1">
-        <f>O18</f>
+        <f t="shared" si="8"/>
         <v>90</v>
       </c>
     </row>
@@ -2428,24 +2477,24 @@
         <v>5</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E21" s="1">
         <f>E20</f>
-        <v>88.25</v>
+        <v>208.25</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>140</v>
       </c>
       <c r="H21" s="1">
         <f>H20</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I21" s="1">
         <f>I20</f>
@@ -2457,21 +2506,21 @@
       </c>
       <c r="K21" s="1">
         <f>H21</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="L21" s="1">
         <v>-25</v>
       </c>
       <c r="M21" s="1">
-        <f>M19</f>
+        <f t="shared" si="8"/>
         <v>288</v>
       </c>
       <c r="N21" s="1">
-        <f>N19</f>
-        <v>92.5</v>
+        <f t="shared" si="8"/>
+        <v>204</v>
       </c>
       <c r="O21" s="1">
-        <f>O19</f>
+        <f t="shared" si="8"/>
         <v>45</v>
       </c>
       <c r="P21" s="1">
@@ -2480,7 +2529,7 @@
       </c>
       <c r="Q21" s="1">
         <f>Q19</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
       <c r="R21" s="1">
         <f>R19</f>
@@ -2498,7 +2547,7 @@
         <v>4</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E22" s="1">
@@ -2506,16 +2555,16 @@
         <v>182.25</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>140</v>
       </c>
       <c r="H22" s="1">
         <f>H15</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I22" s="1">
         <v>25</v>
@@ -2526,7 +2575,7 @@
       </c>
       <c r="K22" s="1">
         <f>RawPoints!H29</f>
-        <v>264.43</v>
+        <v>83.57</v>
       </c>
       <c r="L22" s="1">
         <v>-25</v>
@@ -2537,7 +2586,7 @@
       </c>
       <c r="N22" s="1">
         <f>RawPoints!H30</f>
-        <v>252.43</v>
+        <v>71.569999999999993</v>
       </c>
       <c r="O22" s="1">
         <v>-90</v>
@@ -2554,7 +2603,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E23" s="1">
@@ -2562,7 +2611,7 @@
         <v>182.25</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G23" s="1">
@@ -2571,7 +2620,7 @@
       </c>
       <c r="H23" s="1">
         <f>H22</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I23" s="1">
         <f>I22</f>
@@ -2583,7 +2632,7 @@
       </c>
       <c r="K23" s="1">
         <f>H23</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="L23" s="1">
         <v>-25</v>
@@ -2594,7 +2643,7 @@
       </c>
       <c r="N23" s="1">
         <f>RawPoints!H33</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
       <c r="O23" s="1">
         <v>-90</v>
@@ -2605,7 +2654,7 @@
       </c>
       <c r="Q23" s="1">
         <f>N23</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
       <c r="R23" s="1">
         <v>0</v>
@@ -2622,24 +2671,24 @@
         <v>4</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E24" s="1">
         <f>E16</f>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>140</v>
       </c>
       <c r="H24" s="1">
         <f>H23</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I24" s="1">
         <f>I23</f>
@@ -2651,7 +2700,7 @@
       </c>
       <c r="K24" s="1">
         <f>K22</f>
-        <v>264.43</v>
+        <v>83.57</v>
       </c>
       <c r="L24" s="1">
         <v>-75</v>
@@ -2662,7 +2711,7 @@
       </c>
       <c r="N24" s="1">
         <f>N22</f>
-        <v>252.43</v>
+        <v>71.569999999999993</v>
       </c>
       <c r="O24" s="1">
         <v>-90</v>
@@ -2679,24 +2728,24 @@
         <v>5</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E25" s="1">
         <f>E24</f>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>140</v>
       </c>
       <c r="H25" s="1">
         <f>H24</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I25" s="1">
         <f>I24</f>
@@ -2708,7 +2757,7 @@
       </c>
       <c r="K25" s="1">
         <f>H25</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="L25" s="1">
         <v>-75</v>
@@ -2719,7 +2768,7 @@
       </c>
       <c r="N25" s="1">
         <f>N23</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
       <c r="O25" s="1">
         <f>O23</f>
@@ -2731,7 +2780,7 @@
       </c>
       <c r="Q25" s="1">
         <f>Q23</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
       <c r="R25" s="1">
         <f>R23</f>
@@ -2749,12 +2798,12 @@
         <v>5</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E26" s="1">
         <f>E18</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -2765,7 +2814,7 @@
       </c>
       <c r="H26" s="1">
         <f>H20</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I26" s="1">
         <v>-25</v>
@@ -2776,7 +2825,7 @@
       </c>
       <c r="K26" s="1">
         <f>H26</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="L26" s="1">
         <v>25</v>
@@ -2787,7 +2836,7 @@
       </c>
       <c r="N26" s="1">
         <f>N23</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
       <c r="O26" s="1">
         <v>-25</v>
@@ -2798,7 +2847,7 @@
       </c>
       <c r="Q26" s="1">
         <f>Q25</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
       <c r="R26" s="1">
         <f>R25</f>
@@ -2816,23 +2865,23 @@
         <v>5</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E27" s="1">
         <f>E26</f>
-        <v>43.75</v>
+        <v>307.75</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" ref="G27:G29" si="7">G26</f>
+        <f t="shared" ref="G27:G29" si="9">G26</f>
         <v>140</v>
       </c>
       <c r="H27" s="1">
         <f>H26</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="I27" s="1">
         <v>-25</v>
@@ -2843,7 +2892,7 @@
       </c>
       <c r="K27" s="1">
         <f>H27</f>
-        <v>57.25</v>
+        <v>210.75</v>
       </c>
       <c r="L27" s="1">
         <v>25</v>
@@ -2854,7 +2903,7 @@
       </c>
       <c r="N27" s="1">
         <f>N26</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
       <c r="O27" s="1">
         <v>-25</v>
@@ -2865,7 +2914,7 @@
       </c>
       <c r="Q27" s="1">
         <f>Q26</f>
-        <v>230.18</v>
+        <v>121.32</v>
       </c>
       <c r="R27" s="1">
         <f>R26</f>
@@ -2883,34 +2932,34 @@
         <v>5</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E28" s="1">
         <f>E24</f>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
       </c>
       <c r="G28" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>140</v>
       </c>
       <c r="H28" s="1">
         <f>H25</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I28" s="1">
         <v>25</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" ref="J28:J29" si="8">J27</f>
+        <f t="shared" ref="J28:J29" si="10">J27</f>
         <v>228.75</v>
       </c>
       <c r="K28" s="1">
         <f>K23</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="L28" s="1">
         <v>-25</v>
@@ -2921,7 +2970,7 @@
       </c>
       <c r="N28" s="1">
         <f>N21</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
       <c r="O28" s="1">
         <v>25</v>
@@ -2932,7 +2981,7 @@
       </c>
       <c r="Q28" s="1">
         <f>Q21</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
       <c r="R28" s="1">
         <v>0</v>
@@ -2949,35 +2998,35 @@
         <v>5</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="E29" s="1">
         <f>E25</f>
-        <v>244.25</v>
+        <v>16.25</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
       </c>
       <c r="G29" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>140</v>
       </c>
       <c r="H29" s="1">
         <f>H28</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="I29" s="1">
         <f>I25</f>
         <v>25</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>228.75</v>
       </c>
       <c r="K29" s="1">
         <f>H29</f>
-        <v>230.75</v>
+        <v>113.25</v>
       </c>
       <c r="L29" s="1">
         <f>L28</f>
@@ -2989,7 +3038,7 @@
       </c>
       <c r="N29" s="1">
         <f>N28</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
       <c r="O29" s="1">
         <v>25</v>
@@ -3000,7 +3049,7 @@
       </c>
       <c r="Q29" s="1">
         <f>N29</f>
-        <v>92.5</v>
+        <v>204</v>
       </c>
       <c r="R29" s="1">
         <v>0</v>
@@ -3037,10 +3086,10 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B31" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -3055,12 +3104,41 @@
         <v>0</v>
       </c>
       <c r="G31" s="1">
+        <v>96</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
         <v>120</v>
       </c>
-      <c r="H31" s="1">
-        <v>0</v>
-      </c>
-      <c r="I31" s="1">
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>